<commit_message>
REST, DATABASE and KAFKA Example added
</commit_message>
<xml_diff>
--- a/rest-db-kafka/src/test/resources/virtualan_collection_kafka_db_testcase_0.xlsx
+++ b/rest-db-kafka/src/test/resources/virtualan_collection_kafka_db_testcase_0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\jan-release\asyncapi-virtualization\idaithalam-kafka\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\jan-release\idaithalam\samples\idaithalam-db-kafka-apitesting\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D0E6DC-8A32-477A-B852-307634A160DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F7869C-7D59-4912-B3F1-81BC1FCD53A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,17 +206,17 @@
     <t>tag=grey</t>
   </si>
   <si>
-    <t>petId=100</t>
-  </si>
-  <si>
-    <t>name=Rocky</t>
-  </si>
-  <si>
-    <t>id,name, category/id:name,status
-i~101,Rockey,i~100:german shepherd,available</t>
-  </si>
-  <si>
     <t>VERIFY</t>
+  </si>
+  <si>
+    <t>petId=1000</t>
+  </si>
+  <si>
+    <t>id,name,category/id:name,status
+i~1000,doggie,i~1000:Rocky,available</t>
+  </si>
+  <si>
+    <t>name=doggie</t>
   </si>
 </sst>
 </file>
@@ -285,13 +285,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,8 +524,8 @@
   </sheetPr>
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -533,7 +536,7 @@
     <col min="7" max="7" width="24.42578125" customWidth="1"/>
     <col min="10" max="10" width="68.42578125" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="15" max="15" width="68" customWidth="1"/>
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -630,14 +633,14 @@
       <c r="N2" t="s">
         <v>46</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="S2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -657,16 +660,16 @@
         <v>8</v>
       </c>
       <c r="N3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>62</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="Q3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R3">
         <v>200</v>
@@ -823,7 +826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -839,11 +842,11 @@
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="P9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with KAFKA TESTING EXAMPLE
</commit_message>
<xml_diff>
--- a/rest-db-kafka/src/test/resources/virtualan_collection_kafka_db_testcase_0.xlsx
+++ b/rest-db-kafka/src/test/resources/virtualan_collection_kafka_db_testcase_0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\jan-release\idaithalam\samples\idaithalam-db-kafka-apitesting\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED9433-08C1-440F-9A4D-C94481D6D3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3D5966-2B04-4F66-B2D5-28B3969D9706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API-Testing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -180,94 +180,89 @@
     <t>tag=grey</t>
   </si>
   <si>
-    <t>petId=100</t>
-  </si>
-  <si>
-    <t>name=Rocky</t>
+    <t>VERIFY</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>DB_INSERT</t>
+  </si>
+  <si>
+    <t>DB_VERIFY</t>
+  </si>
+  <si>
+    <t>SEND_KAFKA</t>
+  </si>
+  <si>
+    <t>VERIFY_KAFKA</t>
+  </si>
+  <si>
+    <t>REST_GET_1</t>
+  </si>
+  <si>
+    <t>REST_GET_2</t>
+  </si>
+  <si>
+    <t>REST_POST</t>
+  </si>
+  <si>
+    <t>DB_CREATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from employees where emp_no = 1
+EMP_NO,BIRTH_DATE,FIRST_NAME,LAST_NAME,GENDER,HIRE_DATE
+i~1,l~253087200000,ELan,Thangamani,Male,l~1191992400000          </t>
+  </si>
+  <si>
+    <t>petId=1000</t>
+  </si>
+  <si>
+    <t>name=doggie</t>
   </si>
   <si>
     <t>id,name, category/id:name,status
-i~101,Rockey,i~100:german shepherd,available</t>
-  </si>
-  <si>
-    <t>VERIFY</t>
-  </si>
-  <si>
-    <t>employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMP_NO,BIRTH_DATE,FIRST_NAME,LAST_NAME,GENDER,HIRE_DATE
-i~1,l~253087200000,ELan,Thangamani,Male,l~1191992400000          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">select * from employees where emp_no = 1 </t>
-  </si>
-  <si>
-    <t>DB_INSERT</t>
-  </si>
-  <si>
-    <t>DB_VERIFY</t>
-  </si>
-  <si>
-    <t>SEND_KAFKA</t>
-  </si>
-  <si>
-    <t>VERIFY_KAFKA</t>
-  </si>
-  <si>
-    <t>REST_GET_1</t>
-  </si>
-  <si>
-    <t>REST_GET_2</t>
-  </si>
-  <si>
-    <t>REST_POST</t>
-  </si>
-  <si>
-    <t>DB_CREATE</t>
+i~1000,doggie,i~1000:Rocky,available</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <color theme="3"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF008000"/>
-      <name val="Consolas"/>
-    </font>
-    <font>
-      <b/>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF1155CC"/>
-      <name val="Inconsolata"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,13 +275,40 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -295,14 +317,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +555,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -555,26 +577,26 @@
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
@@ -583,283 +605,358 @@
       <c r="I1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>35</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>100</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S2" t="s">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" t="s">
-        <v>54</v>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3">
+      <c r="Q3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="1">
         <v>200</v>
       </c>
+      <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="R4" s="1">
         <v>200</v>
       </c>
+      <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="Q5" s="1"/>
       <c r="R5" s="1">
         <v>200</v>
       </c>
+      <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>100</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S6" t="s">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J7" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="P7" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:19" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J8" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="P8" t="s">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J9" t="s">
-        <v>58</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="P9" t="s">
-        <v>55</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2">

</xml_diff>